<commit_message>
Update ECE Parts Order Form
</commit_message>
<xml_diff>
--- a/Logistics/ECE_Parts Order Form_75.xlsx
+++ b/Logistics/ECE_Parts Order Form_75.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="78">
   <si>
     <t>Team #:</t>
   </si>
@@ -63,9 +63,6 @@
   </si>
   <si>
     <t>Phone: ________________</t>
-  </si>
-  <si>
-    <t>Website: ____________________________________________</t>
   </si>
   <si>
     <t>Fax: ____________________</t>
@@ -215,33 +212,15 @@
     <t>Pack of 100</t>
   </si>
   <si>
-    <t>Butt Splice Connector, 26-22 Wire Size</t>
-  </si>
-  <si>
     <t>E-FFR250N-100 </t>
   </si>
   <si>
     <t>22/18-Gauge Female Quick Disconnects</t>
   </si>
   <si>
-    <t>Name: __Amazon_________________________</t>
-  </si>
-  <si>
     <t>Name: __McMaster Carr_________________________</t>
   </si>
   <si>
-    <t>10 Feet</t>
-  </si>
-  <si>
-    <t>8233T31</t>
-  </si>
-  <si>
-    <t>22 Gauge, 2 Conductor Wire</t>
-  </si>
-  <si>
-    <t>http://www.mcmaster.com/#8233t31/=thugyo</t>
-  </si>
-  <si>
     <t>3 ft USB to RS232</t>
   </si>
   <si>
@@ -254,18 +233,12 @@
     <t>6459K29</t>
   </si>
   <si>
-    <t>86825K745</t>
-  </si>
-  <si>
     <t>LME12UU</t>
   </si>
   <si>
     <t>http://www.amazonsupply.com/lme12uu-linear-motion-bushings-closed/dp/B002BBJUIO</t>
   </si>
   <si>
-    <t>http://www.amazonsupply.com/dp/B005GDFFKQ?ref_=sr_1_5_txt</t>
-  </si>
-  <si>
     <t>http://www.amazonsupply.com/dp/B00M4D0DU8?ref_=sr_1_1_txt</t>
   </si>
   <si>
@@ -281,12 +254,6 @@
     <t>Hardened Precision 400 Series Stainless Steel Metric Shaft, 12 mm Diameter, 1200 mm Length</t>
   </si>
   <si>
-    <t>Machinable Multipurpose MIC6 Cast Aluminum, Precision-Ground Sheet, 5/16" Thick, 12" x 12"</t>
-  </si>
-  <si>
-    <t>http://www.mcmaster.com/#86825k745/=tjut1o</t>
-  </si>
-  <si>
     <t>http://www.mcmaster.com/#6459k29/=tjuslw</t>
   </si>
   <si>
@@ -294,6 +261,12 @@
   </si>
   <si>
     <t>Website: _____http://www.mcmaster.com_______________________________________</t>
+  </si>
+  <si>
+    <t>Name: __Amazon Supply_________________________</t>
+  </si>
+  <si>
+    <t>Website: __http://www.amazonsupply.com__________________________________________</t>
   </si>
 </sst>
 </file>
@@ -376,7 +349,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -433,19 +406,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
@@ -463,7 +423,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -535,25 +495,18 @@
       <alignment readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" readingOrder="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" readingOrder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1011,10 +964,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I100"/>
+  <dimension ref="A1:I97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="E97" sqref="E97"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H70" sqref="H70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1031,15 +984,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="7" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="42" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
+      <c r="A1" s="45" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
       <c r="H1" s="28"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -1060,7 +1013,7 @@
       </c>
       <c r="C4" s="4"/>
       <c r="E4" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -1073,12 +1026,12 @@
       <c r="A6" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="41">
+      <c r="B6" s="39">
         <v>41884</v>
       </c>
       <c r="C6" s="4"/>
       <c r="E6" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -1093,13 +1046,13 @@
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="F8" s="24" t="s">
         <v>24</v>
-      </c>
-      <c r="F8" s="24" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -1110,14 +1063,14 @@
     </row>
     <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
       <c r="D10" s="9"/>
       <c r="E10" s="33">
-        <f>SUM(G19,G37,G53,G71,G89)</f>
-        <v>524.63</v>
+        <f>SUM(G19,G37,G53,G70,G86)</f>
+        <v>379.15</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -1143,10 +1096,10 @@
         <v>8</v>
       </c>
       <c r="H13" s="30" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I13" s="30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -1157,13 +1110,13 @@
         <v>1</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D14" s="34">
         <v>50</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F14" s="25">
         <v>24.95</v>
@@ -1176,7 +1129,7 @@
         <v>41887</v>
       </c>
       <c r="I14" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -1187,13 +1140,13 @@
         <v>1</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D15" s="34">
         <v>1438</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F15" s="21">
         <v>19.95</v>
@@ -1206,7 +1159,7 @@
         <v>41887</v>
       </c>
       <c r="I15" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -1217,13 +1170,13 @@
         <v>2</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D16" s="34">
         <v>324</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F16" s="25">
         <v>14</v>
@@ -1236,7 +1189,7 @@
         <v>41887</v>
       </c>
       <c r="I16" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
@@ -1247,13 +1200,13 @@
         <v>1</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D17" s="34">
         <v>85</v>
       </c>
       <c r="E17" s="17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F17" s="25">
         <v>1.95</v>
@@ -1266,7 +1219,7 @@
         <v>41887</v>
       </c>
       <c r="I17" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
@@ -1277,13 +1230,13 @@
         <v>1</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D18" s="34">
         <v>798</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F18" s="25">
         <v>8.9499999999999993</v>
@@ -1296,7 +1249,7 @@
         <v>41887</v>
       </c>
       <c r="I18" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
@@ -1306,7 +1259,7 @@
       <c r="D19" s="13"/>
       <c r="E19" s="14"/>
       <c r="F19" s="26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G19" s="22">
         <f>SUM(G14:G18)</f>
@@ -1334,13 +1287,13 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
       <c r="E24" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
@@ -1356,7 +1309,7 @@
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
@@ -1370,21 +1323,21 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
       <c r="E28" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F31" s="27" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
@@ -1410,10 +1363,10 @@
         <v>8</v>
       </c>
       <c r="H33" s="30" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I33" s="30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
@@ -1424,13 +1377,13 @@
         <v>1</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D34" s="34">
         <v>5438</v>
       </c>
       <c r="E34" s="17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F34" s="25">
         <v>1.02</v>
@@ -1443,7 +1396,7 @@
         <v>41887</v>
       </c>
       <c r="I34" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
@@ -1454,13 +1407,13 @@
         <v>2</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D35" s="36">
         <v>3726</v>
       </c>
       <c r="E35" s="16" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="F35" s="25">
         <v>5.71</v>
@@ -1473,7 +1426,7 @@
         <v>41887</v>
       </c>
       <c r="I35" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
@@ -1484,13 +1437,13 @@
         <v>2</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D36" s="37">
         <v>3871</v>
       </c>
       <c r="E36" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F36" s="25">
         <v>3.82</v>
@@ -1503,7 +1456,7 @@
         <v>41887</v>
       </c>
       <c r="I36" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
@@ -1513,7 +1466,7 @@
       <c r="D37" s="13"/>
       <c r="E37" s="14"/>
       <c r="F37" s="26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G37" s="22">
         <f>SUM(G34:G36)</f>
@@ -1541,13 +1494,13 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
       <c r="E42" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
@@ -1563,7 +1516,7 @@
       </c>
       <c r="B44" s="4"/>
       <c r="C44" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
@@ -1577,21 +1530,21 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
       <c r="D46" s="4"/>
       <c r="E46" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F49" s="27" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
@@ -1617,10 +1570,10 @@
         <v>8</v>
       </c>
       <c r="H51" s="30" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I51" s="30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
@@ -1631,13 +1584,13 @@
         <v>1</v>
       </c>
       <c r="C52" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D52" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="D52" s="35" t="s">
-        <v>53</v>
-      </c>
       <c r="E52" s="16" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="F52" s="25">
         <v>45</v>
@@ -1650,7 +1603,7 @@
         <v>41887</v>
       </c>
       <c r="I52" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
@@ -1660,7 +1613,7 @@
       <c r="D53" s="13"/>
       <c r="E53" s="14"/>
       <c r="F53" s="26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G53" s="22">
         <f>SUM(G52:G52)</f>
@@ -1688,13 +1641,13 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
       <c r="D58" s="4"/>
       <c r="E58" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
@@ -1710,7 +1663,7 @@
       </c>
       <c r="B60" s="4"/>
       <c r="C60" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D60" s="4"/>
       <c r="E60" s="4"/>
@@ -1724,21 +1677,21 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
       <c r="D62" s="4"/>
       <c r="E62" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F65" s="27" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
@@ -1764,40 +1717,40 @@
         <v>8</v>
       </c>
       <c r="H67" s="30" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I67" s="30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A68" s="38">
+      <c r="A68" s="1">
         <v>12</v>
       </c>
-      <c r="B68" s="38">
+      <c r="B68" s="1">
         <v>1</v>
       </c>
       <c r="C68" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="D68" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="D68" s="38">
-        <v>12142</v>
-      </c>
-      <c r="E68" s="38" t="s">
+      <c r="E68" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="F68" s="39">
-        <v>18.48</v>
+      <c r="F68" s="25">
+        <v>7.98</v>
       </c>
       <c r="G68" s="21">
-        <f t="shared" ref="G68:G70" si="3">(B68*F68)</f>
-        <v>18.48</v>
+        <f t="shared" ref="G68:G69" si="3">(B68*F68)</f>
+        <v>7.98</v>
       </c>
       <c r="H68" s="31">
         <v>41887</v>
       </c>
-      <c r="I68" s="40" t="s">
-        <v>76</v>
+      <c r="I68" s="15" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
@@ -1807,359 +1760,277 @@
       <c r="B69" s="1">
         <v>1</v>
       </c>
-      <c r="C69" s="38" t="s">
-        <v>59</v>
+      <c r="C69" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="D69" s="35" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="E69" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="F69" s="25">
-        <v>7.98</v>
+        <v>74</v>
+      </c>
+      <c r="F69" s="21">
+        <v>24.81</v>
       </c>
       <c r="G69" s="21">
         <f t="shared" si="3"/>
-        <v>7.98</v>
+        <v>24.81</v>
       </c>
       <c r="H69" s="31">
         <v>41887</v>
       </c>
-      <c r="I69" s="15" t="s">
+      <c r="I69" s="11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A70" s="12"/>
+      <c r="B70" s="12"/>
+      <c r="C70" s="12"/>
+      <c r="D70" s="13"/>
+      <c r="E70" s="12"/>
+      <c r="F70" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="G70" s="42">
+        <f>SUM(G68:G69)</f>
+        <v>32.79</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A72" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B72" s="5"/>
+      <c r="C72" s="5"/>
+      <c r="D72" s="5"/>
+      <c r="E72" s="5"/>
+      <c r="F72" s="23"/>
+      <c r="G72" s="23"/>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A74" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B74" s="4"/>
+      <c r="C74" s="4"/>
+      <c r="D74" s="4"/>
+      <c r="E74" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A70" s="1"/>
-      <c r="B70" s="1">
-        <v>1</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D70" s="35" t="s">
-        <v>74</v>
-      </c>
-      <c r="E70" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="F70" s="21">
-        <v>24.81</v>
-      </c>
-      <c r="G70" s="21">
-        <f t="shared" si="3"/>
-        <v>24.81</v>
-      </c>
-      <c r="H70" s="31"/>
-      <c r="I70" s="11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A71" s="12"/>
-      <c r="B71" s="12"/>
-      <c r="C71" s="12"/>
-      <c r="D71" s="13"/>
-      <c r="E71" s="12"/>
-      <c r="F71" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="G71" s="45">
-        <f>SUM(G68:G69)</f>
-        <v>26.46</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A73" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B73" s="5"/>
-      <c r="C73" s="5"/>
-      <c r="D73" s="5"/>
-      <c r="E73" s="5"/>
-      <c r="F73" s="23"/>
-      <c r="G73" s="23"/>
-    </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A75" s="4" t="s">
-        <v>63</v>
-      </c>
+      <c r="A75" s="4"/>
       <c r="B75" s="4"/>
       <c r="C75" s="4"/>
       <c r="D75" s="4"/>
-      <c r="E75" s="4" t="s">
-        <v>13</v>
-      </c>
+      <c r="E75" s="4"/>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A76" s="4"/>
+      <c r="A76" s="4" t="s">
+        <v>9</v>
+      </c>
       <c r="B76" s="4"/>
-      <c r="C76" s="4"/>
+      <c r="C76" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="D76" s="4"/>
       <c r="E76" s="4"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A77" s="4" t="s">
-        <v>9</v>
-      </c>
+      <c r="A77" s="4"/>
       <c r="B77" s="4"/>
-      <c r="C77" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="C77" s="4"/>
       <c r="D77" s="4"/>
       <c r="E77" s="4"/>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A78" s="4"/>
+      <c r="A78" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="B78" s="4"/>
       <c r="C78" s="4"/>
       <c r="D78" s="4"/>
-      <c r="E78" s="4"/>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A79" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B79" s="4"/>
-      <c r="C79" s="4"/>
-      <c r="D79" s="4"/>
-      <c r="E79" s="4" t="s">
+      <c r="E78" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A81" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F81" s="27" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A82" s="4" t="s">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A83" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F83" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G83" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="H83" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="F82" s="27" t="s">
+      <c r="I83" s="30" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A84" s="1">
+        <v>14</v>
+      </c>
+      <c r="B84" s="1">
+        <v>1</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D84" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="E84" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="F84" s="21">
+        <v>58.88</v>
+      </c>
+      <c r="G84" s="21">
+        <f t="shared" ref="G84:G85" si="4">(B84*F84)</f>
+        <v>58.88</v>
+      </c>
+      <c r="H84" s="43">
+        <v>41887</v>
+      </c>
+      <c r="I84" s="11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A85" s="1">
         <v>15</v>
       </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A84" s="2" t="s">
+      <c r="B85" s="1">
         <v>2</v>
       </c>
-      <c r="B84" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C84" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D84" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E84" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F84" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="G84" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="H84" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="I84" s="30" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A85" s="38">
-        <v>14</v>
-      </c>
-      <c r="B85" s="38">
-        <v>1</v>
-      </c>
-      <c r="C85" s="38" t="s">
+      <c r="C85" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D85" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="D85" s="38" t="s">
-        <v>66</v>
-      </c>
-      <c r="E85" s="46" t="s">
-        <v>67</v>
-      </c>
-      <c r="F85" s="39">
-        <v>7.96</v>
+      <c r="E85" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="F85" s="21">
+        <v>69.3</v>
       </c>
       <c r="G85" s="21">
-        <f t="shared" ref="G85:G88" si="4">(B85*F85)</f>
-        <v>7.96</v>
-      </c>
-      <c r="H85" s="47">
-        <v>41887</v>
-      </c>
-      <c r="I85" s="40" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A86" s="1">
-        <v>15</v>
-      </c>
-      <c r="B86" s="1">
-        <v>1</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D86" s="35" t="s">
-        <v>71</v>
-      </c>
-      <c r="E86" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="F86" s="21">
-        <v>58.88</v>
-      </c>
-      <c r="G86" s="21">
-        <f t="shared" si="4"/>
-        <v>58.88</v>
-      </c>
-      <c r="H86" s="47">
-        <v>41887</v>
-      </c>
-      <c r="I86" s="11" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A87" s="1"/>
-      <c r="B87" s="1">
-        <v>2</v>
-      </c>
-      <c r="C87" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="D87" s="35" t="s">
-        <v>72</v>
-      </c>
-      <c r="E87" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="F87" s="21">
-        <v>69.3</v>
-      </c>
-      <c r="G87" s="21">
         <f t="shared" si="4"/>
         <v>138.6</v>
       </c>
-      <c r="H87" s="47">
+      <c r="H85" s="43">
         <v>41887</v>
       </c>
-      <c r="I87" s="11" t="s">
-        <v>84</v>
-      </c>
+      <c r="I85" s="11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B86" s="40"/>
+      <c r="D86" s="41"/>
+      <c r="F86" s="44" t="s">
+        <v>15</v>
+      </c>
+      <c r="G86" s="21">
+        <f>SUM(G84:G85)</f>
+        <v>197.48</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B87" s="40"/>
+      <c r="D87" s="41"/>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A88" s="1"/>
-      <c r="B88" s="49">
-        <v>3</v>
-      </c>
-      <c r="C88" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="D88" s="50" t="s">
-        <v>73</v>
-      </c>
-      <c r="E88" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="F88" s="21">
-        <v>47.95</v>
-      </c>
-      <c r="G88" s="21">
-        <f t="shared" si="4"/>
-        <v>143.85000000000002</v>
-      </c>
-      <c r="H88" s="47">
-        <v>41887</v>
-      </c>
-      <c r="I88" s="11" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B89" s="43"/>
-      <c r="D89" s="44"/>
-      <c r="F89" s="48" t="s">
-        <v>16</v>
-      </c>
-      <c r="G89" s="21">
-        <f>SUM(G85:G88)</f>
-        <v>349.29</v>
-      </c>
+      <c r="A88" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B88" s="5"/>
+      <c r="C88" s="5"/>
+      <c r="D88" s="5"/>
+      <c r="E88" s="5"/>
+      <c r="F88" s="23"/>
+      <c r="G88" s="23"/>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B90" s="43"/>
-      <c r="D90" s="44"/>
+      <c r="A90" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B90" s="4"/>
+      <c r="C90" s="4"/>
+      <c r="D90" s="4"/>
+      <c r="E90" s="4" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A91" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B91" s="5"/>
-      <c r="C91" s="5"/>
-      <c r="D91" s="5"/>
-      <c r="E91" s="5"/>
-      <c r="F91" s="23"/>
-      <c r="G91" s="23"/>
+      <c r="A91" s="4"/>
+      <c r="B91" s="4"/>
+      <c r="C91" s="4"/>
+      <c r="D91" s="4"/>
+      <c r="E91" s="4"/>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A92" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B92" s="4"/>
+      <c r="C92" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D92" s="4"/>
+      <c r="E92" s="4"/>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A93" s="4" t="s">
-        <v>64</v>
-      </c>
+      <c r="A93" s="4"/>
       <c r="B93" s="4"/>
       <c r="C93" s="4"/>
       <c r="D93" s="4"/>
-      <c r="E93" s="4" t="s">
-        <v>86</v>
-      </c>
+      <c r="E93" s="4"/>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A94" s="4"/>
+      <c r="A94" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="B94" s="4"/>
       <c r="C94" s="4"/>
       <c r="D94" s="4"/>
-      <c r="E94" s="4"/>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A95" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B95" s="4"/>
-      <c r="C95" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D95" s="4"/>
-      <c r="E95" s="4"/>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A96" s="4"/>
-      <c r="B96" s="4"/>
-      <c r="C96" s="4"/>
-      <c r="D96" s="4"/>
-      <c r="E96" s="4"/>
+      <c r="E94" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B97" s="4"/>
-      <c r="C97" s="4"/>
-      <c r="D97" s="4"/>
-      <c r="E97" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F97" s="27" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A100" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F100" s="27" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -2178,18 +2049,15 @@
     <hyperlink ref="I35" r:id="rId8"/>
     <hyperlink ref="I34" r:id="rId9"/>
     <hyperlink ref="I52" r:id="rId10"/>
-    <hyperlink ref="I85" r:id="rId11" location="8233t31/=thugyo"/>
-    <hyperlink ref="I70" r:id="rId12"/>
-    <hyperlink ref="I68" r:id="rId13"/>
-    <hyperlink ref="I69" r:id="rId14"/>
-    <hyperlink ref="I86" r:id="rId15" location="7549k1/=tjuroh"/>
-    <hyperlink ref="I88" r:id="rId16" location="86825k745/=tjut1o"/>
-    <hyperlink ref="I87" r:id="rId17" location="6459k29/=tjuslw"/>
+    <hyperlink ref="I69" r:id="rId11"/>
+    <hyperlink ref="I68" r:id="rId12"/>
+    <hyperlink ref="I84" r:id="rId13" location="7549k1/=tjuroh"/>
+    <hyperlink ref="I85" r:id="rId14" location="6459k29/=tjuslw"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="landscape" r:id="rId18"/>
+  <pageSetup orientation="landscape" r:id="rId15"/>
   <headerFooter alignWithMargins="0"/>
-  <drawing r:id="rId19"/>
+  <drawing r:id="rId16"/>
 </worksheet>
 </file>
 

</xml_diff>